<commit_message>
correction of upload end user excel sheet
</commit_message>
<xml_diff>
--- a/api/uploads/END_USERS.xlsx
+++ b/api/uploads/END_USERS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t xml:space="preserve">MNG001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yakshitha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ykmangalore100@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YK001</t>
   </si>
 </sst>
 </file>
@@ -158,10 +167,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -205,9 +214,21 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="jayashree.cs16@sahyadri.edu.in"/>
+    <hyperlink ref="B4" r:id="rId2" display="ykmangalore100@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>